<commit_message>
TMNT - more files
</commit_message>
<xml_diff>
--- a/TMNT/FrameCompare.xlsx
+++ b/TMNT/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\TMNT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F57263-782A-4B90-8499-4D19DA73F2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB86AD0-624D-49D6-806F-60A2F3B2CA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41490" yWindow="120" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Place</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Enter Sewer</t>
+  </si>
+  <si>
+    <t>X = 24</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -705,12 +708,18 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2">
+        <v>927</v>
+      </c>
+      <c r="C6" s="2">
+        <v>927</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">

</xml_diff>